<commit_message>
Berhasil Write Data Gardu
Berhasil write ke excel idpel dan nomor gardu pelanggan
</commit_message>
<xml_diff>
--- a/data/datameter.xlsx
+++ b/data/datameter.xlsx
@@ -1,69 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\GitHub\AMI_Scraper\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACEB350C-D2AD-421E-A2EF-D1518E3B15BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="summary" sheetId="1" r:id="rId1"/>
-    <sheet name="list" sheetId="2" r:id="rId2"/>
+    <sheet name="summary" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="list" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>jumlahbaris</t>
-  </si>
-  <si>
-    <t>nomormeter</t>
-  </si>
-  <si>
-    <t>idpel</t>
-  </si>
-  <si>
-    <t>nomorgardu</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -82,25 +47,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -366,27 +390,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
+    <col width="10.90625" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>jumlahbaris</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2">
         <f>COUNT(list!A:A)</f>
-        <v>20</v>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -395,189 +425,284 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col width="11.81640625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="15.453125" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="11.26953125" bestFit="1" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2">
+    <row r="1" customFormat="1" s="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>nomormeter</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>idpel</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>nomorgardu</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>45610205228</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="2" t="n">
         <v>321201077406</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>GD321111305</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>45610199317</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="2" t="n">
         <v>321209062502</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4">
+    <row r="4">
+      <c r="A4" t="n">
         <v>45610199059</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="2" t="n">
         <v>321201156674</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>GD321110238</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
         <v>45610198466</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="2" t="n">
         <v>321209511422</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>GD321111305</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
         <v>45610165333</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="2" t="n">
         <v>321202675139</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7">
+    <row r="7">
+      <c r="A7" t="n">
         <v>45610205681</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="2" t="n">
         <v>321202659879</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>GD321110218</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
         <v>45610205250</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="2" t="n">
         <v>321209101792</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>GD321110250</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
         <v>45610204833</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="2" t="n">
         <v>321201567823</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>GD321110218</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
         <v>45610205187</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="2" t="n">
         <v>321203215181</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11">
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>GD321110218</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
         <v>45610167786</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="2" t="n">
         <v>321209067254</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>GD321110250</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
         <v>45610199318</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="2" t="n">
         <v>321209035655</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13">
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>GD321110245</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
         <v>45610201715</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="2" t="n">
         <v>321200681314</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14">
+    <row r="14">
+      <c r="A14" t="n">
         <v>45610204890</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="2" t="n">
         <v>321200723467</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15">
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>GD321110246</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
         <v>45610134616</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="2" t="n">
         <v>321201436827</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16">
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>GD321111229</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
         <v>45610153686</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="2" t="n">
         <v>321201007127</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17">
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>GD321110245</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
         <v>45610159263</v>
       </c>
-      <c r="B17" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18">
+      <c r="B17" s="2" t="n">
+        <v>321202683391</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>GD321110218</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
         <v>45610198295</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="2" t="n">
         <v>321209023464</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19">
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>GD321110246</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
         <v>45610197512</v>
       </c>
-      <c r="B19" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20">
+      <c r="B19" s="2" t="n">
+        <v>321201219746</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>GD321110218</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
         <v>45610205629</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="2" t="n">
         <v>321200897965</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21">
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>GD321110246</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
         <v>45610161269</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="2" t="n">
         <v>321209061281</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>GD321110246</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>